<commit_message>
Now working, fix a lot of things
1. voltage max is changed, infeasible, model is relaxed.
</commit_message>
<xml_diff>
--- a/two_stage_D_OPF/temp_results/boundary_variables_iterations.xlsx
+++ b/two_stage_D_OPF/temp_results/boundary_variables_iterations.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,13 +491,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="C2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="D2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -523,28 +523,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="C3" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="D3" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="E3" t="n">
-        <v>359.2200000000051</v>
+        <v>359.220000000004</v>
       </c>
       <c r="F3" t="n">
-        <v>82.02000000000116</v>
+        <v>82.02000000000092</v>
       </c>
       <c r="G3" t="n">
-        <v>323.6200000000045</v>
+        <v>323.6200000000035</v>
       </c>
       <c r="H3" t="n">
         <v>179.6</v>
       </c>
       <c r="I3" t="n">
-        <v>41.01000000000058</v>
+        <v>41.01000000000046</v>
       </c>
       <c r="J3" t="n">
         <v>161.8100000000022</v>
@@ -555,16 +555,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="C4" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="D4" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="E4" t="n">
-        <v>844.4900000000295</v>
+        <v>844.4900000000283</v>
       </c>
       <c r="F4" t="n">
         <v>529.05</v>
@@ -573,10 +573,10 @@
         <v>697.0800000000231</v>
       </c>
       <c r="H4" t="n">
-        <v>460.1900000000167</v>
+        <v>460.190000000016</v>
       </c>
       <c r="I4" t="n">
-        <v>322.6400000000152</v>
+        <v>322.6400000000148</v>
       </c>
       <c r="J4" t="n">
         <v>369.6700000000128</v>
@@ -587,13 +587,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="C5" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="D5" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="E5" t="n">
         <v>1266.520000000063</v>
@@ -608,7 +608,7 @@
         <v>676.5200000000341</v>
       </c>
       <c r="I5" t="n">
-        <v>530.9900000000334</v>
+        <v>530.9900000000332</v>
       </c>
       <c r="J5" t="n">
         <v>563.7100000000282</v>
@@ -619,13 +619,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="C6" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="D6" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="E6" t="n">
         <v>1408.090000000055</v>
@@ -651,16 +651,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="C7" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="D7" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="E7" t="n">
-        <v>1408.090000000055</v>
+        <v>1408.090000000052</v>
       </c>
       <c r="F7" t="n">
         <v>950.35</v>
@@ -672,42 +672,10 @@
         <v>747.3</v>
       </c>
       <c r="I7" t="n">
-        <v>570.9900000000333</v>
+        <v>570.9900000000436</v>
       </c>
       <c r="J7" t="n">
-        <v>613.7100000000282</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1408.090000000055</v>
-      </c>
-      <c r="F8" t="n">
-        <v>950.35</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1153.1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>747.3</v>
-      </c>
-      <c r="I8" t="n">
-        <v>570.9900000000333</v>
-      </c>
-      <c r="J8" t="n">
-        <v>613.7100000000282</v>
+        <v>613.7100000000355</v>
       </c>
     </row>
   </sheetData>
@@ -721,7 +689,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -781,13 +749,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="C2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="D2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="E2" t="n">
         <v>359.22</v>
@@ -796,7 +764,7 @@
         <v>82.02000000000001</v>
       </c>
       <c r="G2" t="n">
-        <v>323.62</v>
+        <v>323.6199999999999</v>
       </c>
       <c r="H2" t="n">
         <v>179.6</v>
@@ -805,7 +773,7 @@
         <v>41.01000000000001</v>
       </c>
       <c r="J2" t="n">
-        <v>161.81</v>
+        <v>161.8100000000004</v>
       </c>
     </row>
     <row r="3">
@@ -813,31 +781,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="C3" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="D3" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="E3" t="n">
-        <v>844.4900000000183</v>
+        <v>844.4900000000181</v>
       </c>
       <c r="F3" t="n">
         <v>529.05</v>
       </c>
       <c r="G3" t="n">
-        <v>697.0800000000138</v>
+        <v>697.0800000000148</v>
       </c>
       <c r="H3" t="n">
         <v>460.1900000000105</v>
       </c>
       <c r="I3" t="n">
-        <v>322.6400000000109</v>
+        <v>322.640000000011</v>
       </c>
       <c r="J3" t="n">
-        <v>369.6700000000079</v>
+        <v>369.6700000000083</v>
       </c>
     </row>
     <row r="4">
@@ -845,16 +813,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.049999901141005</v>
+        <v>1.029999899221413</v>
       </c>
       <c r="C4" t="n">
-        <v>1.049999977427301</v>
+        <v>1.029999976988996</v>
       </c>
       <c r="D4" t="n">
-        <v>1.049999910936636</v>
+        <v>1.02999990920725</v>
       </c>
       <c r="E4" t="n">
-        <v>1266.520000000044</v>
+        <v>1266.520000000043</v>
       </c>
       <c r="F4" t="n">
         <v>870.35</v>
@@ -866,7 +834,7 @@
         <v>676.5200000000236</v>
       </c>
       <c r="I4" t="n">
-        <v>530.9900000000252</v>
+        <v>530.990000000025</v>
       </c>
       <c r="J4" t="n">
         <v>563.7100000000196</v>
@@ -877,13 +845,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.049999760626254</v>
+        <v>1.029999755978219</v>
       </c>
       <c r="C5" t="n">
-        <v>1.049999843737761</v>
+        <v>1.029999840703543</v>
       </c>
       <c r="D5" t="n">
-        <v>1.049999804280024</v>
+        <v>1.029999800479636</v>
       </c>
       <c r="E5" t="n">
         <v>1408.090000000043</v>
@@ -909,16 +877,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.049999643504316</v>
+        <v>1.029999636582067</v>
       </c>
       <c r="C6" t="n">
-        <v>1.049999742891738</v>
+        <v>1.029999737899343</v>
       </c>
       <c r="D6" t="n">
-        <v>1.049999703358772</v>
+        <v>1.029999697598747</v>
       </c>
       <c r="E6" t="n">
-        <v>1408.090000000043</v>
+        <v>1408.090000000033</v>
       </c>
       <c r="F6" t="n">
         <v>950.35</v>
@@ -930,10 +898,10 @@
         <v>747.3</v>
       </c>
       <c r="I6" t="n">
-        <v>570.9900000000285</v>
+        <v>570.9900000000358</v>
       </c>
       <c r="J6" t="n">
-        <v>613.7100000000232</v>
+        <v>613.7100000000273</v>
       </c>
     </row>
     <row r="7">
@@ -941,13 +909,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.049999604543784</v>
+        <v>1.029999596865019</v>
       </c>
       <c r="C7" t="n">
-        <v>1.049999720874957</v>
+        <v>1.029999715455052</v>
       </c>
       <c r="D7" t="n">
-        <v>1.049999675837795</v>
+        <v>1.029999669543382</v>
       </c>
       <c r="E7" t="n">
         <v>1408.090000000043</v>
@@ -965,38 +933,6 @@
         <v>570.9900000000285</v>
       </c>
       <c r="J7" t="n">
-        <v>613.7100000000232</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1.049999604543784</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1.049999720874957</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1.049999675837795</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1408.090000000043</v>
-      </c>
-      <c r="F8" t="n">
-        <v>950.35</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1153.1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>747.3</v>
-      </c>
-      <c r="I8" t="n">
-        <v>570.9900000000285</v>
-      </c>
-      <c r="J8" t="n">
         <v>613.7100000000232</v>
       </c>
     </row>
@@ -1011,7 +947,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1071,13 +1007,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="C2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="D2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="E2" t="n">
         <v>203.85</v>
@@ -1103,16 +1039,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.042612493602766</v>
+        <v>1.022468000387581</v>
       </c>
       <c r="C3" t="n">
-        <v>1.052941474009921</v>
+        <v>1.032998423494961</v>
       </c>
       <c r="D3" t="n">
-        <v>1.040538614018013</v>
+        <v>1.02035317770982</v>
       </c>
       <c r="E3" t="n">
-        <v>625.8800000000098</v>
+        <v>625.8800000000097</v>
       </c>
       <c r="F3" t="n">
         <v>513.4200000000078</v>
@@ -1135,31 +1071,31 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.027014649413675</v>
+        <v>1.006558041103589</v>
       </c>
       <c r="C4" t="n">
-        <v>1.043256222673312</v>
+        <v>1.023124404042142</v>
       </c>
       <c r="D4" t="n">
-        <v>1.032688797100925</v>
+        <v>1.012346853434017</v>
       </c>
       <c r="E4" t="n">
         <v>767.45</v>
       </c>
       <c r="F4" t="n">
-        <v>593.4200000000078</v>
+        <v>593.420000000008</v>
       </c>
       <c r="G4" t="n">
-        <v>629.3600000000084</v>
+        <v>629.3600000000085</v>
       </c>
       <c r="H4" t="n">
-        <v>412.3400000000053</v>
+        <v>412.3400000000054</v>
       </c>
       <c r="I4" t="n">
         <v>339.5700000000047</v>
       </c>
       <c r="J4" t="n">
-        <v>326.8200000000045</v>
+        <v>326.8200000000046</v>
       </c>
     </row>
     <row r="5">
@@ -1167,31 +1103,31 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.015051202829744</v>
+        <v>0.9943485024708942</v>
       </c>
       <c r="C5" t="n">
-        <v>1.036772529160841</v>
+        <v>1.016512310413684</v>
       </c>
       <c r="D5" t="n">
-        <v>1.02344966468987</v>
+        <v>1.002920343872736</v>
       </c>
       <c r="E5" t="n">
         <v>767.45</v>
       </c>
       <c r="F5" t="n">
-        <v>593.4200000000078</v>
+        <v>593.4200000000278</v>
       </c>
       <c r="G5" t="n">
-        <v>629.3600000000084</v>
+        <v>629.36000000003</v>
       </c>
       <c r="H5" t="n">
-        <v>412.3400000000053</v>
+        <v>412.340000000019</v>
       </c>
       <c r="I5" t="n">
-        <v>339.5700000000047</v>
+        <v>339.5700000000164</v>
       </c>
       <c r="J5" t="n">
-        <v>326.8200000000045</v>
+        <v>326.8200000000161</v>
       </c>
     </row>
     <row r="6">
@@ -1199,31 +1135,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.010765420433047</v>
+        <v>0.9899730981916601</v>
       </c>
       <c r="C6" t="n">
-        <v>1.036397478379902</v>
+        <v>1.016129781667785</v>
       </c>
       <c r="D6" t="n">
-        <v>1.020595629739161</v>
+        <v>1.00000771969154</v>
       </c>
       <c r="E6" t="n">
         <v>767.45</v>
       </c>
       <c r="F6" t="n">
-        <v>593.4200000000078</v>
+        <v>593.420000000008</v>
       </c>
       <c r="G6" t="n">
-        <v>629.3600000000084</v>
+        <v>629.3600000000085</v>
       </c>
       <c r="H6" t="n">
-        <v>412.3400000000053</v>
+        <v>412.3400000000054</v>
       </c>
       <c r="I6" t="n">
         <v>339.5700000000047</v>
       </c>
       <c r="J6" t="n">
-        <v>326.8200000000045</v>
+        <v>326.8200000000046</v>
       </c>
     </row>
     <row r="7">
@@ -1231,63 +1167,31 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.010765298764849</v>
+        <v>0.9899729739680746</v>
       </c>
       <c r="C7" t="n">
-        <v>1.036397376210309</v>
+        <v>1.016129677460319</v>
       </c>
       <c r="D7" t="n">
-        <v>1.020595525910287</v>
+        <v>1.000007613725063</v>
       </c>
       <c r="E7" t="n">
         <v>767.45</v>
       </c>
       <c r="F7" t="n">
-        <v>593.4200000000078</v>
+        <v>593.420000000008</v>
       </c>
       <c r="G7" t="n">
-        <v>629.3600000000084</v>
+        <v>629.3600000000085</v>
       </c>
       <c r="H7" t="n">
-        <v>412.3400000000053</v>
+        <v>412.3400000000054</v>
       </c>
       <c r="I7" t="n">
         <v>339.5700000000047</v>
       </c>
       <c r="J7" t="n">
-        <v>326.8200000000045</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1.010765258292006</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1.036397353904565</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1.020595497596408</v>
-      </c>
-      <c r="E8" t="n">
-        <v>767.45</v>
-      </c>
-      <c r="F8" t="n">
-        <v>593.4200000000078</v>
-      </c>
-      <c r="G8" t="n">
-        <v>629.3600000000084</v>
-      </c>
-      <c r="H8" t="n">
-        <v>412.3400000000053</v>
-      </c>
-      <c r="I8" t="n">
-        <v>339.5700000000047</v>
-      </c>
-      <c r="J8" t="n">
-        <v>326.8200000000045</v>
+        <v>326.8200000000046</v>
       </c>
     </row>
   </sheetData>
@@ -1301,7 +1205,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1361,13 +1265,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="C2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="D2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="E2" t="n">
         <v>422.03</v>
@@ -1393,13 +1297,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.044613367904488</v>
+        <v>1.024508217831734</v>
       </c>
       <c r="C3" t="n">
-        <v>1.044031778070914</v>
+        <v>1.023915208218881</v>
       </c>
       <c r="D3" t="n">
-        <v>1.044427776245559</v>
+        <v>1.02431898186023</v>
       </c>
       <c r="E3" t="n">
         <v>563.6</v>
@@ -1425,13 +1329,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.020477541930996</v>
+        <v>0.9998872004308923</v>
       </c>
       <c r="C4" t="n">
-        <v>1.034509034730744</v>
+        <v>1.014203597998166</v>
       </c>
       <c r="D4" t="n">
-        <v>1.021729663342779</v>
+        <v>1.001165073778819</v>
       </c>
       <c r="E4" t="n">
         <v>563.6</v>
@@ -1457,13 +1361,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9983143113597298</v>
+        <v>0.9772571126707913</v>
       </c>
       <c r="C5" t="n">
-        <v>1.023227705513918</v>
+        <v>1.002693840277917</v>
       </c>
       <c r="D5" t="n">
-        <v>1.009510485204314</v>
+        <v>0.9886917718568555</v>
       </c>
       <c r="E5" t="n">
         <v>563.6</v>
@@ -1489,13 +1393,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9860026970153114</v>
+        <v>0.9646767948496874</v>
       </c>
       <c r="C6" t="n">
-        <v>1.016616283760621</v>
+        <v>0.9959461172208336</v>
       </c>
       <c r="D6" t="n">
-        <v>1.000057240478515</v>
+        <v>0.9790375295327033</v>
       </c>
       <c r="E6" t="n">
         <v>563.6</v>
@@ -1521,63 +1425,31 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9815900922984868</v>
+        <v>0.9601661883749877</v>
       </c>
       <c r="C7" t="n">
-        <v>1.016233794152168</v>
+        <v>0.9955556862259944</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9971362532384268</v>
+        <v>0.9760536396747709</v>
       </c>
       <c r="E7" t="n">
-        <v>563.6</v>
+        <v>478.0899354777617</v>
       </c>
       <c r="F7" t="n">
-        <v>421.3</v>
+        <v>372.9789915816977</v>
       </c>
       <c r="G7" t="n">
-        <v>456.02</v>
+        <v>395.6187394771221</v>
       </c>
       <c r="H7" t="n">
-        <v>287.11</v>
+        <v>244.357987801907</v>
       </c>
       <c r="I7" t="n">
-        <v>248.35</v>
+        <v>224.1894957908488</v>
       </c>
       <c r="J7" t="n">
-        <v>244.04</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.981589967014003</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1.016233689955367</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.9971361469667965</v>
-      </c>
-      <c r="E8" t="n">
-        <v>563.6</v>
-      </c>
-      <c r="F8" t="n">
-        <v>421.3</v>
-      </c>
-      <c r="G8" t="n">
-        <v>456.02</v>
-      </c>
-      <c r="H8" t="n">
-        <v>287.11</v>
-      </c>
-      <c r="I8" t="n">
-        <v>248.35</v>
-      </c>
-      <c r="J8" t="n">
-        <v>244.04</v>
+        <v>213.8393697385611</v>
       </c>
     </row>
   </sheetData>
@@ -1591,7 +1463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1651,13 +1523,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="C2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="D2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="E2" t="n">
         <v>141.57</v>
@@ -1683,13 +1555,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.047175579929618</v>
+        <v>1.02712058454737</v>
       </c>
       <c r="C3" t="n">
-        <v>1.047269726176925</v>
+        <v>1.027216568872743</v>
       </c>
       <c r="D3" t="n">
-        <v>1.046871166622804</v>
+        <v>1.026810225653305</v>
       </c>
       <c r="E3" t="n">
         <v>141.57</v>
@@ -1715,13 +1587,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.039975704415729</v>
+        <v>1.019779125975322</v>
       </c>
       <c r="C4" t="n">
-        <v>1.040703425957213</v>
+        <v>1.020521251826379</v>
       </c>
       <c r="D4" t="n">
-        <v>1.039811090255206</v>
+        <v>1.019611249557229</v>
       </c>
       <c r="E4" t="n">
         <v>141.57</v>
@@ -1747,13 +1619,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.015729683998535</v>
+        <v>0.9950411001339402</v>
       </c>
       <c r="C5" t="n">
-        <v>1.031149945505842</v>
+        <v>1.010777032782102</v>
       </c>
       <c r="D5" t="n">
-        <v>1.017009945172132</v>
+        <v>0.9963479455386173</v>
       </c>
       <c r="E5" t="n">
         <v>141.57</v>
@@ -1779,13 +1651,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9934605385398486</v>
+        <v>0.9722982266958458</v>
       </c>
       <c r="C6" t="n">
-        <v>1.019831458873693</v>
+        <v>0.9992278064278642</v>
       </c>
       <c r="D6" t="n">
-        <v>1.004733369288552</v>
+        <v>0.9838135714463</v>
       </c>
       <c r="E6" t="n">
         <v>141.57</v>
@@ -1811,16 +1683,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9810880163836996</v>
+        <v>0.9596529038624853</v>
       </c>
       <c r="C7" t="n">
-        <v>1.013197875829012</v>
+        <v>0.992456518047324</v>
       </c>
       <c r="D7" t="n">
-        <v>0.995234750125807</v>
+        <v>0.9741109833371012</v>
       </c>
       <c r="E7" t="n">
-        <v>141.57</v>
+        <v>101.57</v>
       </c>
       <c r="F7" t="n">
         <v>80</v>
@@ -1829,44 +1701,12 @@
         <v>100</v>
       </c>
       <c r="H7" t="n">
-        <v>70.78</v>
+        <v>50.78</v>
       </c>
       <c r="I7" t="n">
         <v>40</v>
       </c>
       <c r="J7" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.9766532069618091</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1.012814095258392</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.9922995672410847</v>
-      </c>
-      <c r="E8" t="n">
-        <v>141.57</v>
-      </c>
-      <c r="F8" t="n">
-        <v>80</v>
-      </c>
-      <c r="G8" t="n">
-        <v>100</v>
-      </c>
-      <c r="H8" t="n">
-        <v>70.78</v>
-      </c>
-      <c r="I8" t="n">
-        <v>40</v>
-      </c>
-      <c r="J8" t="n">
         <v>50</v>
       </c>
     </row>
@@ -1881,7 +1721,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1941,13 +1781,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="C2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="D2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -1973,13 +1813,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.044613367904488</v>
+        <v>1.024508217831734</v>
       </c>
       <c r="C3" t="n">
-        <v>1.044031778070914</v>
+        <v>1.023915208218881</v>
       </c>
       <c r="D3" t="n">
-        <v>1.044427776245559</v>
+        <v>1.02431898186023</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -2005,13 +1845,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.02047755399942</v>
+        <v>0.9998872127478373</v>
       </c>
       <c r="C4" t="n">
-        <v>1.034509044981132</v>
+        <v>1.014203608453777</v>
       </c>
       <c r="D4" t="n">
-        <v>1.021729673729116</v>
+        <v>1.001165084378498</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -2037,13 +1877,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.998314327799759</v>
+        <v>0.9772571294650578</v>
       </c>
       <c r="C5" t="n">
-        <v>1.023227718139864</v>
+        <v>1.002693853162426</v>
       </c>
       <c r="D5" t="n">
-        <v>1.009510498582979</v>
+        <v>0.9886917855172327</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -2069,13 +1909,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9860027136606172</v>
+        <v>0.9646768118629674</v>
       </c>
       <c r="C6" t="n">
-        <v>1.016616296468678</v>
+        <v>0.9959461301926376</v>
       </c>
       <c r="D6" t="n">
-        <v>1.000057253983644</v>
+        <v>0.9790375433277848</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -2101,13 +1941,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9815901090186193</v>
+        <v>0.9601662054681915</v>
       </c>
       <c r="C7" t="n">
-        <v>1.016233806865008</v>
+        <v>0.9955556992028856</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9971362667831178</v>
+        <v>0.9760536535120252</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -2125,38 +1965,6 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.9815899837341377</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1.016233702668209</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.997136160511489</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2171,7 +1979,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2231,16 +2039,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="C2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="D2" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="E2" t="n">
-        <v>281.42</v>
+        <v>281.4199999999997</v>
       </c>
       <c r="F2" t="n">
         <v>274.91</v>
@@ -2263,16 +2071,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.039149644425647</v>
+        <v>1.018936692591816</v>
       </c>
       <c r="C3" t="n">
-        <v>1.054045827194369</v>
+        <v>1.034124074315433</v>
       </c>
       <c r="D3" t="n">
-        <v>1.037055340417739</v>
+        <v>1.016800756829455</v>
       </c>
       <c r="E3" t="n">
-        <v>281.42</v>
+        <v>281.4199999999997</v>
       </c>
       <c r="F3" t="n">
         <v>274.91</v>
@@ -2295,16 +2103,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.018461728207205</v>
+        <v>0.9978297910078687</v>
       </c>
       <c r="C4" t="n">
-        <v>1.039087101971659</v>
+        <v>1.018872909387555</v>
       </c>
       <c r="D4" t="n">
-        <v>1.025416306336036</v>
+        <v>1.004927162186314</v>
       </c>
       <c r="E4" t="n">
-        <v>281.42</v>
+        <v>281.4199999999997</v>
       </c>
       <c r="F4" t="n">
         <v>274.91</v>
@@ -2327,16 +2135,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.006396626936783</v>
+        <v>0.9855121362569483</v>
       </c>
       <c r="C5" t="n">
-        <v>1.032577240582067</v>
+        <v>1.012233055065915</v>
       </c>
       <c r="D5" t="n">
-        <v>1.016111060376742</v>
+        <v>0.9954304029011509</v>
       </c>
       <c r="E5" t="n">
-        <v>281.42</v>
+        <v>281.4199999999997</v>
       </c>
       <c r="F5" t="n">
         <v>274.91</v>
@@ -2359,16 +2167,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.002073834445516</v>
+        <v>0.9810973293615369</v>
       </c>
       <c r="C6" t="n">
-        <v>1.032200667684307</v>
+        <v>1.011848910839918</v>
       </c>
       <c r="D6" t="n">
-        <v>1.013236357468761</v>
+        <v>0.9924958015511011</v>
       </c>
       <c r="E6" t="n">
-        <v>281.42</v>
+        <v>281.4199999999997</v>
       </c>
       <c r="F6" t="n">
         <v>274.91</v>
@@ -2391,16 +2199,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.002073711722017</v>
+        <v>0.9810972040141283</v>
       </c>
       <c r="C7" t="n">
-        <v>1.032200565099303</v>
+        <v>1.011848806191577</v>
       </c>
       <c r="D7" t="n">
-        <v>1.013236252885763</v>
+        <v>0.9924956947825938</v>
       </c>
       <c r="E7" t="n">
-        <v>281.42</v>
+        <v>281.4199999999997</v>
       </c>
       <c r="F7" t="n">
         <v>274.91</v>
@@ -2415,38 +2223,6 @@
         <v>190.41</v>
       </c>
       <c r="J7" t="n">
-        <v>125.08</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1.002073670898129</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1.032200542702867</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1.013236224366237</v>
-      </c>
-      <c r="E8" t="n">
-        <v>281.42</v>
-      </c>
-      <c r="F8" t="n">
-        <v>274.91</v>
-      </c>
-      <c r="G8" t="n">
-        <v>200.12</v>
-      </c>
-      <c r="H8" t="n">
-        <v>155.36</v>
-      </c>
-      <c r="I8" t="n">
-        <v>190.41</v>
-      </c>
-      <c r="J8" t="n">
         <v>125.08</v>
       </c>
     </row>

</xml_diff>

<commit_message>
now working perfectly and giving expected output after including CLPU and model update only while solving.
</commit_message>
<xml_diff>
--- a/two_stage_D_OPF/temp_results/boundary_variables_iterations.xlsx
+++ b/two_stage_D_OPF/temp_results/boundary_variables_iterations.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,13 +491,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="C2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="D2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -523,31 +523,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="C3" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="D3" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="E3" t="n">
-        <v>359.220000000004</v>
+        <v>364.4442298107892</v>
       </c>
       <c r="F3" t="n">
-        <v>82.02000000000092</v>
+        <v>83.58726894323006</v>
       </c>
       <c r="G3" t="n">
-        <v>323.6200000000035</v>
+        <v>328.8442298107799</v>
       </c>
       <c r="H3" t="n">
-        <v>179.6</v>
+        <v>185.6076679312938</v>
       </c>
       <c r="I3" t="n">
-        <v>41.01000000000046</v>
+        <v>47.01766793125782</v>
       </c>
       <c r="J3" t="n">
-        <v>161.8100000000022</v>
+        <v>167.8176679312892</v>
       </c>
     </row>
     <row r="4">
@@ -555,31 +555,31 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="C4" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="D4" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="E4" t="n">
-        <v>844.4900000000283</v>
+        <v>857.5505745270177</v>
       </c>
       <c r="F4" t="n">
-        <v>529.05</v>
+        <v>536.8863447162646</v>
       </c>
       <c r="G4" t="n">
-        <v>697.0800000000231</v>
+        <v>706.4836136594666</v>
       </c>
       <c r="H4" t="n">
-        <v>460.190000000016</v>
+        <v>473.0509457457053</v>
       </c>
       <c r="I4" t="n">
-        <v>322.6400000000148</v>
+        <v>318.4734559158753</v>
       </c>
       <c r="J4" t="n">
-        <v>369.6700000000128</v>
+        <v>400.5561630795419</v>
       </c>
     </row>
     <row r="5">
@@ -587,31 +587,31 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="C5" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="D5" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="E5" t="n">
-        <v>1266.520000000063</v>
+        <v>1284.804804337769</v>
       </c>
       <c r="F5" t="n">
-        <v>870.35</v>
+        <v>882.8881515459391</v>
       </c>
       <c r="G5" t="n">
-        <v>1053.1</v>
+        <v>1067.20542048914</v>
       </c>
       <c r="H5" t="n">
-        <v>676.5200000000341</v>
+        <v>714.3311635725458</v>
       </c>
       <c r="I5" t="n">
-        <v>530.9900000000332</v>
+        <v>514.8555114989493</v>
       </c>
       <c r="J5" t="n">
-        <v>563.7100000000282</v>
+        <v>602.3561751221714</v>
       </c>
     </row>
     <row r="6">
@@ -619,31 +619,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="C6" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="D6" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="E6" t="n">
-        <v>1408.090000000055</v>
+        <v>1429.121146832115</v>
       </c>
       <c r="F6" t="n">
-        <v>950.35</v>
+        <v>963.9329975081139</v>
       </c>
       <c r="G6" t="n">
-        <v>1153.1</v>
+        <v>1168.772689432398</v>
       </c>
       <c r="H6" t="n">
-        <v>747.3</v>
+        <v>787.7902639129366</v>
       </c>
       <c r="I6" t="n">
-        <v>570.9900000000333</v>
+        <v>557.5346118393204</v>
       </c>
       <c r="J6" t="n">
-        <v>613.7100000000282</v>
+        <v>655.0352754625492</v>
       </c>
     </row>
     <row r="7">
@@ -651,31 +651,63 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="C7" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="D7" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="E7" t="n">
-        <v>1408.090000000052</v>
+        <v>1429.121146832115</v>
       </c>
       <c r="F7" t="n">
-        <v>950.35</v>
+        <v>963.9329975081139</v>
       </c>
       <c r="G7" t="n">
-        <v>1153.1</v>
+        <v>1168.772689432398</v>
       </c>
       <c r="H7" t="n">
-        <v>747.3</v>
+        <v>787.7902639129366</v>
       </c>
       <c r="I7" t="n">
-        <v>570.9900000000436</v>
+        <v>557.5346118393204</v>
       </c>
       <c r="J7" t="n">
-        <v>613.7100000000355</v>
+        <v>655.0352754625492</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1429.121146832115</v>
+      </c>
+      <c r="F8" t="n">
+        <v>963.9329975081139</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1168.772689432398</v>
+      </c>
+      <c r="H8" t="n">
+        <v>787.7902639129366</v>
+      </c>
+      <c r="I8" t="n">
+        <v>557.5346118393204</v>
+      </c>
+      <c r="J8" t="n">
+        <v>655.0352754625492</v>
       </c>
     </row>
   </sheetData>
@@ -689,7 +721,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -749,31 +781,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="C2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="D2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="E2" t="n">
-        <v>359.22</v>
+        <v>364.4442298106945</v>
       </c>
       <c r="F2" t="n">
-        <v>82.02000000000001</v>
+        <v>83.58726894320836</v>
       </c>
       <c r="G2" t="n">
-        <v>323.6199999999999</v>
+        <v>328.8442298106945</v>
       </c>
       <c r="H2" t="n">
-        <v>179.6</v>
+        <v>185.6076679312456</v>
       </c>
       <c r="I2" t="n">
-        <v>41.01000000000001</v>
+        <v>47.01766793124562</v>
       </c>
       <c r="J2" t="n">
-        <v>161.8100000000004</v>
+        <v>167.8176679312456</v>
       </c>
     </row>
     <row r="3">
@@ -781,31 +813,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="C3" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="D3" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="E3" t="n">
-        <v>844.4900000000181</v>
+        <v>857.5505745269245</v>
       </c>
       <c r="F3" t="n">
-        <v>529.05</v>
+        <v>536.8863447162062</v>
       </c>
       <c r="G3" t="n">
-        <v>697.0800000000148</v>
+        <v>706.4836136593898</v>
       </c>
       <c r="H3" t="n">
-        <v>460.1900000000105</v>
+        <v>473.0509457456538</v>
       </c>
       <c r="I3" t="n">
-        <v>322.640000000011</v>
+        <v>318.4734559158407</v>
       </c>
       <c r="J3" t="n">
-        <v>369.6700000000083</v>
+        <v>400.5561630794983</v>
       </c>
     </row>
     <row r="4">
@@ -813,31 +845,31 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.029999899221413</v>
+        <v>1.039999898109871</v>
       </c>
       <c r="C4" t="n">
-        <v>1.029999976988996</v>
+        <v>1.039999975807095</v>
       </c>
       <c r="D4" t="n">
-        <v>1.02999990920725</v>
+        <v>1.039999907999691</v>
       </c>
       <c r="E4" t="n">
-        <v>1266.520000000043</v>
+        <v>1284.804804337676</v>
       </c>
       <c r="F4" t="n">
-        <v>870.35</v>
+        <v>882.8881515458755</v>
       </c>
       <c r="G4" t="n">
-        <v>1053.1</v>
+        <v>1067.205420489063</v>
       </c>
       <c r="H4" t="n">
-        <v>676.5200000000236</v>
+        <v>714.3311635724945</v>
       </c>
       <c r="I4" t="n">
-        <v>530.990000000025</v>
+        <v>514.8555114989122</v>
       </c>
       <c r="J4" t="n">
-        <v>563.7100000000196</v>
+        <v>602.3561751221279</v>
       </c>
     </row>
     <row r="5">
@@ -845,31 +877,31 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.029999755978219</v>
+        <v>1.03999975352295</v>
       </c>
       <c r="C5" t="n">
-        <v>1.029999840703543</v>
+        <v>1.039999841555456</v>
       </c>
       <c r="D5" t="n">
-        <v>1.029999800479636</v>
+        <v>1.03999979493493</v>
       </c>
       <c r="E5" t="n">
-        <v>1408.090000000043</v>
+        <v>1429.12114683202</v>
       </c>
       <c r="F5" t="n">
-        <v>950.35</v>
+        <v>963.93299750805</v>
       </c>
       <c r="G5" t="n">
-        <v>1153.1</v>
+        <v>1168.77268943232</v>
       </c>
       <c r="H5" t="n">
-        <v>747.3</v>
+        <v>787.7902639128843</v>
       </c>
       <c r="I5" t="n">
-        <v>570.9900000000285</v>
+        <v>557.5346118392833</v>
       </c>
       <c r="J5" t="n">
-        <v>613.7100000000232</v>
+        <v>655.0352754625056</v>
       </c>
     </row>
     <row r="6">
@@ -877,31 +909,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.029999636582067</v>
+        <v>1.039999629685403</v>
       </c>
       <c r="C6" t="n">
-        <v>1.029999737899343</v>
+        <v>1.039999741085718</v>
       </c>
       <c r="D6" t="n">
-        <v>1.029999697598747</v>
+        <v>1.039999690734887</v>
       </c>
       <c r="E6" t="n">
-        <v>1408.090000000033</v>
+        <v>1429.12114683202</v>
       </c>
       <c r="F6" t="n">
-        <v>950.35</v>
+        <v>963.93299750805</v>
       </c>
       <c r="G6" t="n">
-        <v>1153.1</v>
+        <v>1168.77268943232</v>
       </c>
       <c r="H6" t="n">
-        <v>747.3</v>
+        <v>787.7902639128843</v>
       </c>
       <c r="I6" t="n">
-        <v>570.9900000000358</v>
+        <v>557.5346118392833</v>
       </c>
       <c r="J6" t="n">
-        <v>613.7100000000273</v>
+        <v>655.0352754625056</v>
       </c>
     </row>
     <row r="7">
@@ -909,31 +941,63 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.029999596865019</v>
+        <v>1.039999589345254</v>
       </c>
       <c r="C7" t="n">
-        <v>1.029999715455052</v>
+        <v>1.039999718167423</v>
       </c>
       <c r="D7" t="n">
-        <v>1.029999669543382</v>
+        <v>1.039999662162698</v>
       </c>
       <c r="E7" t="n">
-        <v>1408.090000000043</v>
+        <v>1429.12114683202</v>
       </c>
       <c r="F7" t="n">
-        <v>950.35</v>
+        <v>963.93299750805</v>
       </c>
       <c r="G7" t="n">
-        <v>1153.1</v>
+        <v>1168.77268943232</v>
       </c>
       <c r="H7" t="n">
-        <v>747.3</v>
+        <v>787.7902639128843</v>
       </c>
       <c r="I7" t="n">
-        <v>570.9900000000285</v>
+        <v>557.5346118392833</v>
       </c>
       <c r="J7" t="n">
-        <v>613.7100000000232</v>
+        <v>655.0352754625056</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1.039999589345254</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.039999718167423</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.039999662162698</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1429.12114683202</v>
+      </c>
+      <c r="F8" t="n">
+        <v>963.93299750805</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1168.77268943232</v>
+      </c>
+      <c r="H8" t="n">
+        <v>787.7902639128843</v>
+      </c>
+      <c r="I8" t="n">
+        <v>557.5346118392833</v>
+      </c>
+      <c r="J8" t="n">
+        <v>655.0352754625056</v>
       </c>
     </row>
   </sheetData>
@@ -947,7 +1011,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1007,31 +1071,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="C2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="D2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="E2" t="n">
-        <v>203.85</v>
+        <v>206.9845378864167</v>
       </c>
       <c r="F2" t="n">
-        <v>172.12</v>
+        <v>174.7321149053473</v>
       </c>
       <c r="G2" t="n">
-        <v>173.34</v>
+        <v>174.9072689432084</v>
       </c>
       <c r="H2" t="n">
-        <v>125.23</v>
+        <v>114.6140161473994</v>
       </c>
       <c r="I2" t="n">
-        <v>91.22</v>
+        <v>94.31954910926353</v>
       </c>
       <c r="J2" t="n">
-        <v>82.78</v>
+        <v>99.93145590425594</v>
       </c>
     </row>
     <row r="3">
@@ -1039,31 +1103,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.022468000387581</v>
+        <v>1.032401984112262</v>
       </c>
       <c r="C3" t="n">
-        <v>1.032998423494961</v>
+        <v>1.042882508278693</v>
       </c>
       <c r="D3" t="n">
-        <v>1.02035317770982</v>
+        <v>1.030228570376868</v>
       </c>
       <c r="E3" t="n">
-        <v>625.8800000000097</v>
+        <v>634.2387676971672</v>
       </c>
       <c r="F3" t="n">
-        <v>513.4200000000078</v>
+        <v>520.7339217350176</v>
       </c>
       <c r="G3" t="n">
-        <v>529.3600000000082</v>
+        <v>535.6290757728808</v>
       </c>
       <c r="H3" t="n">
-        <v>341.560000000005</v>
+        <v>355.8942339742388</v>
       </c>
       <c r="I3" t="n">
-        <v>299.5700000000048</v>
+        <v>290.7016046923342</v>
       </c>
       <c r="J3" t="n">
-        <v>276.8200000000045</v>
+        <v>301.7314679468855</v>
       </c>
     </row>
     <row r="4">
@@ -1071,31 +1135,31 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.006558041103589</v>
+        <v>1.016107099765069</v>
       </c>
       <c r="C4" t="n">
-        <v>1.023124404042142</v>
+        <v>1.033866132633719</v>
       </c>
       <c r="D4" t="n">
-        <v>1.012346853434017</v>
+        <v>1.021290314278993</v>
       </c>
       <c r="E4" t="n">
-        <v>767.45</v>
+        <v>778.5551101915065</v>
       </c>
       <c r="F4" t="n">
-        <v>593.420000000008</v>
+        <v>601.7787676971931</v>
       </c>
       <c r="G4" t="n">
-        <v>629.3600000000085</v>
+        <v>637.1963447161371</v>
       </c>
       <c r="H4" t="n">
-        <v>412.3400000000054</v>
+        <v>429.3533343146273</v>
       </c>
       <c r="I4" t="n">
-        <v>339.5700000000047</v>
+        <v>333.3807050327064</v>
       </c>
       <c r="J4" t="n">
-        <v>326.8200000000046</v>
+        <v>354.4105682872632</v>
       </c>
     </row>
     <row r="5">
@@ -1103,31 +1167,31 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9943485024708942</v>
+        <v>1.00271034331611</v>
       </c>
       <c r="C5" t="n">
-        <v>1.016512310413684</v>
+        <v>1.027985207796856</v>
       </c>
       <c r="D5" t="n">
-        <v>1.002920343872736</v>
+        <v>1.011851412025817</v>
       </c>
       <c r="E5" t="n">
-        <v>767.45</v>
+        <v>778.5551101915065</v>
       </c>
       <c r="F5" t="n">
-        <v>593.4200000000278</v>
+        <v>601.7787676971931</v>
       </c>
       <c r="G5" t="n">
-        <v>629.36000000003</v>
+        <v>637.1963447161371</v>
       </c>
       <c r="H5" t="n">
-        <v>412.340000000019</v>
+        <v>429.3533343146273</v>
       </c>
       <c r="I5" t="n">
-        <v>339.5700000000164</v>
+        <v>333.3807050327064</v>
       </c>
       <c r="J5" t="n">
-        <v>326.8200000000161</v>
+        <v>354.4105682872632</v>
       </c>
     </row>
     <row r="6">
@@ -1135,31 +1199,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9899730981916601</v>
+        <v>0.9982657725350382</v>
       </c>
       <c r="C6" t="n">
-        <v>1.016129781667785</v>
+        <v>1.027564933875723</v>
       </c>
       <c r="D6" t="n">
-        <v>1.00000771969154</v>
+        <v>1.008857446454194</v>
       </c>
       <c r="E6" t="n">
-        <v>767.45</v>
+        <v>778.5551101915065</v>
       </c>
       <c r="F6" t="n">
-        <v>593.420000000008</v>
+        <v>601.7787676971931</v>
       </c>
       <c r="G6" t="n">
-        <v>629.3600000000085</v>
+        <v>637.1963447161371</v>
       </c>
       <c r="H6" t="n">
-        <v>412.3400000000054</v>
+        <v>429.3533343146273</v>
       </c>
       <c r="I6" t="n">
-        <v>339.5700000000047</v>
+        <v>333.3807050327064</v>
       </c>
       <c r="J6" t="n">
-        <v>326.8200000000046</v>
+        <v>354.4105682872632</v>
       </c>
     </row>
     <row r="7">
@@ -1167,31 +1231,63 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9899729739680746</v>
+        <v>0.9982656435202785</v>
       </c>
       <c r="C7" t="n">
-        <v>1.016129677460319</v>
+        <v>1.027564832190167</v>
       </c>
       <c r="D7" t="n">
-        <v>1.000007613725063</v>
+        <v>1.008857339037606</v>
       </c>
       <c r="E7" t="n">
-        <v>767.45</v>
+        <v>778.5551101915065</v>
       </c>
       <c r="F7" t="n">
-        <v>593.420000000008</v>
+        <v>601.7787676971931</v>
       </c>
       <c r="G7" t="n">
-        <v>629.3600000000085</v>
+        <v>637.1963447161371</v>
       </c>
       <c r="H7" t="n">
-        <v>412.3400000000054</v>
+        <v>429.3533343146273</v>
       </c>
       <c r="I7" t="n">
-        <v>339.5700000000047</v>
+        <v>333.3807050327064</v>
       </c>
       <c r="J7" t="n">
-        <v>326.8200000000046</v>
+        <v>354.4105682872632</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.99826560149365</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.027564808994531</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.008857309583424</v>
+      </c>
+      <c r="E8" t="n">
+        <v>778.5551101915065</v>
+      </c>
+      <c r="F8" t="n">
+        <v>601.7787676971931</v>
+      </c>
+      <c r="G8" t="n">
+        <v>637.1963447161371</v>
+      </c>
+      <c r="H8" t="n">
+        <v>429.3533343146273</v>
+      </c>
+      <c r="I8" t="n">
+        <v>333.3807050327064</v>
+      </c>
+      <c r="J8" t="n">
+        <v>354.4105682872632</v>
       </c>
     </row>
   </sheetData>
@@ -1205,7 +1301,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1265,31 +1361,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="C2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="D2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="E2" t="n">
-        <v>422.03</v>
+        <v>427.2542298106945</v>
       </c>
       <c r="F2" t="n">
-        <v>341.3</v>
+        <v>346.001806829625</v>
       </c>
       <c r="G2" t="n">
-        <v>356.02</v>
+        <v>360.7218068296251</v>
       </c>
       <c r="H2" t="n">
-        <v>216.33</v>
+        <v>241.2802178268078</v>
       </c>
       <c r="I2" t="n">
-        <v>208.35</v>
+        <v>196.3820555830449</v>
       </c>
       <c r="J2" t="n">
-        <v>194.04</v>
+        <v>201.8000120426031</v>
       </c>
     </row>
     <row r="3">
@@ -1297,31 +1393,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.024508217831734</v>
+        <v>1.035335596345601</v>
       </c>
       <c r="C3" t="n">
-        <v>1.023915208218881</v>
+        <v>1.034109827053007</v>
       </c>
       <c r="D3" t="n">
-        <v>1.02431898186023</v>
+        <v>1.03314219029583</v>
       </c>
       <c r="E3" t="n">
-        <v>563.6</v>
+        <v>571.5705723050305</v>
       </c>
       <c r="F3" t="n">
-        <v>421.3</v>
+        <v>427.0466527918014</v>
       </c>
       <c r="G3" t="n">
-        <v>456.02</v>
+        <v>462.2890757728805</v>
       </c>
       <c r="H3" t="n">
-        <v>287.11</v>
+        <v>314.7393181671952</v>
       </c>
       <c r="I3" t="n">
-        <v>248.35</v>
+        <v>239.061155923418</v>
       </c>
       <c r="J3" t="n">
-        <v>244.04</v>
+        <v>254.4791123829808</v>
       </c>
     </row>
     <row r="4">
@@ -1329,31 +1425,31 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.9998872004308923</v>
+        <v>1.008930802862981</v>
       </c>
       <c r="C4" t="n">
-        <v>1.014203597998166</v>
+        <v>1.025360291534958</v>
       </c>
       <c r="D4" t="n">
-        <v>1.001165073778819</v>
+        <v>1.009834572661229</v>
       </c>
       <c r="E4" t="n">
-        <v>563.6</v>
+        <v>571.5705723050305</v>
       </c>
       <c r="F4" t="n">
-        <v>421.3</v>
+        <v>427.0466527918014</v>
       </c>
       <c r="G4" t="n">
-        <v>456.02</v>
+        <v>462.2890757728805</v>
       </c>
       <c r="H4" t="n">
-        <v>287.11</v>
+        <v>314.7393181671952</v>
       </c>
       <c r="I4" t="n">
-        <v>248.35</v>
+        <v>239.061155923418</v>
       </c>
       <c r="J4" t="n">
-        <v>244.04</v>
+        <v>254.4791123829808</v>
       </c>
     </row>
     <row r="5">
@@ -1361,31 +1457,31 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9772571126707913</v>
+        <v>0.9857906477701217</v>
       </c>
       <c r="C5" t="n">
-        <v>1.002693840277917</v>
+        <v>1.014671910621255</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9886917718568555</v>
+        <v>0.9962772825688997</v>
       </c>
       <c r="E5" t="n">
-        <v>563.6</v>
+        <v>571.5705723050305</v>
       </c>
       <c r="F5" t="n">
-        <v>421.3</v>
+        <v>427.0466527918014</v>
       </c>
       <c r="G5" t="n">
-        <v>456.02</v>
+        <v>462.2890757728805</v>
       </c>
       <c r="H5" t="n">
-        <v>287.11</v>
+        <v>314.7393181671952</v>
       </c>
       <c r="I5" t="n">
-        <v>248.35</v>
+        <v>239.061155923418</v>
       </c>
       <c r="J5" t="n">
-        <v>244.04</v>
+        <v>254.4791123829808</v>
       </c>
     </row>
     <row r="6">
@@ -1393,31 +1489,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9646767948496874</v>
+        <v>0.971976129146784</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9959461172208336</v>
+        <v>1.008679083477956</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9790375295327033</v>
+        <v>0.9865991069028126</v>
       </c>
       <c r="E6" t="n">
-        <v>563.6</v>
+        <v>571.5705723050305</v>
       </c>
       <c r="F6" t="n">
-        <v>421.3</v>
+        <v>427.0466527918014</v>
       </c>
       <c r="G6" t="n">
-        <v>456.02</v>
+        <v>462.2890757728805</v>
       </c>
       <c r="H6" t="n">
-        <v>287.11</v>
+        <v>314.7393181671952</v>
       </c>
       <c r="I6" t="n">
-        <v>248.35</v>
+        <v>239.061155923418</v>
       </c>
       <c r="J6" t="n">
-        <v>244.04</v>
+        <v>254.4791123829808</v>
       </c>
     </row>
     <row r="7">
@@ -1425,31 +1521,63 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9601661883749877</v>
+        <v>0.9673903636345733</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9955556862259944</v>
+        <v>1.008250762126071</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9760536396747709</v>
+        <v>0.9835282736092869</v>
       </c>
       <c r="E7" t="n">
-        <v>478.0899354777617</v>
+        <v>571.5705723050305</v>
       </c>
       <c r="F7" t="n">
-        <v>372.9789915816977</v>
+        <v>427.0466527918014</v>
       </c>
       <c r="G7" t="n">
-        <v>395.6187394771221</v>
+        <v>462.2890757728805</v>
       </c>
       <c r="H7" t="n">
-        <v>244.357987801907</v>
+        <v>314.7393181671952</v>
       </c>
       <c r="I7" t="n">
-        <v>224.1894957908488</v>
+        <v>239.061155923418</v>
       </c>
       <c r="J7" t="n">
-        <v>213.8393697385611</v>
+        <v>254.4791123829808</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.9673902305021542</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.008250658492615</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.9835281634263593</v>
+      </c>
+      <c r="E8" t="n">
+        <v>571.5705723050305</v>
+      </c>
+      <c r="F8" t="n">
+        <v>427.0466527918014</v>
+      </c>
+      <c r="G8" t="n">
+        <v>462.2890757728805</v>
+      </c>
+      <c r="H8" t="n">
+        <v>314.7393181671952</v>
+      </c>
+      <c r="I8" t="n">
+        <v>239.061155923418</v>
+      </c>
+      <c r="J8" t="n">
+        <v>254.4791123829808</v>
       </c>
     </row>
   </sheetData>
@@ -1463,7 +1591,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1523,31 +1651,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="C2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="D2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="E2" t="n">
-        <v>141.57</v>
+        <v>144.3163424942691</v>
       </c>
       <c r="F2" t="n">
-        <v>80</v>
+        <v>81.04484596213891</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>101.5672689432084</v>
       </c>
       <c r="H2" t="n">
-        <v>70.78</v>
+        <v>73.45910034035339</v>
       </c>
       <c r="I2" t="n">
-        <v>40</v>
+        <v>42.67910034035339</v>
       </c>
       <c r="J2" t="n">
-        <v>50</v>
+        <v>52.67910034035339</v>
       </c>
     </row>
     <row r="3">
@@ -1555,31 +1683,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.02712058454737</v>
+        <v>1.036798681002614</v>
       </c>
       <c r="C3" t="n">
-        <v>1.027216568872743</v>
+        <v>1.037410143910582</v>
       </c>
       <c r="D3" t="n">
-        <v>1.026810225653305</v>
+        <v>1.036821274071466</v>
       </c>
       <c r="E3" t="n">
-        <v>141.57</v>
+        <v>144.3163424942691</v>
       </c>
       <c r="F3" t="n">
-        <v>80</v>
+        <v>81.04484596213891</v>
       </c>
       <c r="G3" t="n">
-        <v>100</v>
+        <v>101.5672689432084</v>
       </c>
       <c r="H3" t="n">
-        <v>70.78</v>
+        <v>73.45910034035339</v>
       </c>
       <c r="I3" t="n">
-        <v>40</v>
+        <v>42.67910034035339</v>
       </c>
       <c r="J3" t="n">
-        <v>50</v>
+        <v>52.67910034035339</v>
       </c>
     </row>
     <row r="4">
@@ -1587,31 +1715,31 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.019779125975322</v>
+        <v>1.030256381472678</v>
       </c>
       <c r="C4" t="n">
-        <v>1.020521251826379</v>
+        <v>1.030886979000166</v>
       </c>
       <c r="D4" t="n">
-        <v>1.019611249557229</v>
+        <v>1.028403127038137</v>
       </c>
       <c r="E4" t="n">
-        <v>141.57</v>
+        <v>144.3163424942691</v>
       </c>
       <c r="F4" t="n">
-        <v>80</v>
+        <v>81.04484596213891</v>
       </c>
       <c r="G4" t="n">
-        <v>100</v>
+        <v>101.5672689432084</v>
       </c>
       <c r="H4" t="n">
-        <v>70.78</v>
+        <v>73.45910034035339</v>
       </c>
       <c r="I4" t="n">
-        <v>40</v>
+        <v>42.67910034035339</v>
       </c>
       <c r="J4" t="n">
-        <v>50</v>
+        <v>52.67910034035339</v>
       </c>
     </row>
     <row r="5">
@@ -1619,31 +1747,31 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9950411001339402</v>
+        <v>1.003717978054898</v>
       </c>
       <c r="C5" t="n">
-        <v>1.010777032782102</v>
+        <v>1.022109855407501</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9963479455386173</v>
+        <v>1.004985607098152</v>
       </c>
       <c r="E5" t="n">
-        <v>141.57</v>
+        <v>144.3163424942691</v>
       </c>
       <c r="F5" t="n">
-        <v>80</v>
+        <v>81.04484596213891</v>
       </c>
       <c r="G5" t="n">
-        <v>100</v>
+        <v>101.5672689432084</v>
       </c>
       <c r="H5" t="n">
-        <v>70.78</v>
+        <v>73.45910034035339</v>
       </c>
       <c r="I5" t="n">
-        <v>40</v>
+        <v>42.67910034035339</v>
       </c>
       <c r="J5" t="n">
-        <v>50</v>
+        <v>52.67910034035339</v>
       </c>
     </row>
     <row r="6">
@@ -1651,31 +1779,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9722982266958458</v>
+        <v>0.9804548004553344</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9992278064278642</v>
+        <v>1.011387124333841</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9838135714463</v>
+        <v>0.9913620075912865</v>
       </c>
       <c r="E6" t="n">
-        <v>141.57</v>
+        <v>144.3163424942691</v>
       </c>
       <c r="F6" t="n">
-        <v>80</v>
+        <v>81.04484596213891</v>
       </c>
       <c r="G6" t="n">
-        <v>100</v>
+        <v>101.5672689432084</v>
       </c>
       <c r="H6" t="n">
-        <v>70.78</v>
+        <v>73.45910034035339</v>
       </c>
       <c r="I6" t="n">
-        <v>40</v>
+        <v>42.67910034035339</v>
       </c>
       <c r="J6" t="n">
-        <v>50</v>
+        <v>52.67910034035339</v>
       </c>
     </row>
     <row r="7">
@@ -1683,31 +1811,63 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9596529038624853</v>
+        <v>0.9665640227817499</v>
       </c>
       <c r="C7" t="n">
-        <v>0.992456518047324</v>
+        <v>1.005374717461314</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9741109833371012</v>
+        <v>0.981635372260995</v>
       </c>
       <c r="E7" t="n">
-        <v>101.57</v>
+        <v>144.3163424942691</v>
       </c>
       <c r="F7" t="n">
-        <v>80</v>
+        <v>81.04484596213891</v>
       </c>
       <c r="G7" t="n">
-        <v>100</v>
+        <v>101.5672689432084</v>
       </c>
       <c r="H7" t="n">
-        <v>50.78</v>
+        <v>73.45910034035339</v>
       </c>
       <c r="I7" t="n">
-        <v>40</v>
+        <v>42.67910034035339</v>
       </c>
       <c r="J7" t="n">
-        <v>50</v>
+        <v>52.67910034035339</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.9619524573272348</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.004944987744251</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.9785489621482508</v>
+      </c>
+      <c r="E8" t="n">
+        <v>144.3163424942691</v>
+      </c>
+      <c r="F8" t="n">
+        <v>81.04484596213891</v>
+      </c>
+      <c r="G8" t="n">
+        <v>101.5672689432084</v>
+      </c>
+      <c r="H8" t="n">
+        <v>73.45910034035339</v>
+      </c>
+      <c r="I8" t="n">
+        <v>42.67910034035339</v>
+      </c>
+      <c r="J8" t="n">
+        <v>52.67910034035339</v>
       </c>
     </row>
   </sheetData>
@@ -1721,7 +1881,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1781,13 +1941,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="C2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="D2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -1813,13 +1973,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.024508217831734</v>
+        <v>1.035335596345601</v>
       </c>
       <c r="C3" t="n">
-        <v>1.023915208218881</v>
+        <v>1.034109827053007</v>
       </c>
       <c r="D3" t="n">
-        <v>1.02431898186023</v>
+        <v>1.03314219029583</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -1845,13 +2005,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.9998872127478373</v>
+        <v>1.00893081564651</v>
       </c>
       <c r="C4" t="n">
-        <v>1.014203608453777</v>
+        <v>1.02536030174009</v>
       </c>
       <c r="D4" t="n">
-        <v>1.001165084378498</v>
+        <v>1.009834583407987</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -1877,13 +2037,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9772571294650578</v>
+        <v>0.9857906651157186</v>
       </c>
       <c r="C5" t="n">
-        <v>1.002693853162426</v>
+        <v>1.014671923286314</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9886917855172327</v>
+        <v>0.9962772964488157</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -1909,13 +2069,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9646768118629674</v>
+        <v>0.9719761467389105</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9959461301926376</v>
+        <v>1.008679096218262</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9790375433277848</v>
+        <v>0.9865991209188855</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -1941,13 +2101,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9601662054681915</v>
+        <v>0.9673903813100927</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9955556992028856</v>
+        <v>1.008250774871789</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9760536535120252</v>
+        <v>0.9835282876691216</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -1965,6 +2125,38 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.9673902481776759</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.008250671238334</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.9835281774861957</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1979,7 +2171,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2039,31 +2231,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="C2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="D2" t="n">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="E2" t="n">
-        <v>281.4199999999997</v>
+        <v>286.1218068296328</v>
       </c>
       <c r="F2" t="n">
-        <v>274.91</v>
+        <v>278.5669608674862</v>
       </c>
       <c r="G2" t="n">
-        <v>200.12</v>
+        <v>202.7321149053473</v>
       </c>
       <c r="H2" t="n">
-        <v>155.36</v>
+        <v>172.8292616669041</v>
       </c>
       <c r="I2" t="n">
-        <v>190.41</v>
+        <v>177.136238875234</v>
       </c>
       <c r="J2" t="n">
-        <v>125.08</v>
+        <v>132.8070392439114</v>
       </c>
     </row>
     <row r="3">
@@ -2071,31 +2263,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.018936692591816</v>
+        <v>1.02885677381874</v>
       </c>
       <c r="C3" t="n">
-        <v>1.034124074315433</v>
+        <v>1.043962502032817</v>
       </c>
       <c r="D3" t="n">
-        <v>1.016800756829455</v>
+        <v>1.026622585849494</v>
       </c>
       <c r="E3" t="n">
-        <v>281.4199999999997</v>
+        <v>286.1218068296328</v>
       </c>
       <c r="F3" t="n">
-        <v>274.91</v>
+        <v>278.5669608674862</v>
       </c>
       <c r="G3" t="n">
-        <v>200.12</v>
+        <v>202.7321149053473</v>
       </c>
       <c r="H3" t="n">
-        <v>155.36</v>
+        <v>172.8292616669041</v>
       </c>
       <c r="I3" t="n">
-        <v>190.41</v>
+        <v>177.136238875234</v>
       </c>
       <c r="J3" t="n">
-        <v>125.08</v>
+        <v>132.8070392439114</v>
       </c>
     </row>
     <row r="4">
@@ -2103,31 +2295,31 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.9978297910078687</v>
+        <v>1.006768341793142</v>
       </c>
       <c r="C4" t="n">
-        <v>1.018872909387555</v>
+        <v>1.030089042860626</v>
       </c>
       <c r="D4" t="n">
-        <v>1.004927162186314</v>
+        <v>1.013747060190389</v>
       </c>
       <c r="E4" t="n">
-        <v>281.4199999999997</v>
+        <v>286.1218068296328</v>
       </c>
       <c r="F4" t="n">
-        <v>274.91</v>
+        <v>278.5669608674862</v>
       </c>
       <c r="G4" t="n">
-        <v>200.12</v>
+        <v>202.7321149053473</v>
       </c>
       <c r="H4" t="n">
-        <v>155.36</v>
+        <v>172.8292616669041</v>
       </c>
       <c r="I4" t="n">
-        <v>190.41</v>
+        <v>177.136238875234</v>
       </c>
       <c r="J4" t="n">
-        <v>125.08</v>
+        <v>132.8070392439114</v>
       </c>
     </row>
     <row r="5">
@@ -2135,31 +2327,31 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9855121362569483</v>
+        <v>0.9932456464704157</v>
       </c>
       <c r="C5" t="n">
-        <v>1.012233055065915</v>
+        <v>1.02418644024979</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9954304029011509</v>
+        <v>1.004237271628626</v>
       </c>
       <c r="E5" t="n">
-        <v>281.4199999999997</v>
+        <v>286.1218068296328</v>
       </c>
       <c r="F5" t="n">
-        <v>274.91</v>
+        <v>278.5669608674862</v>
       </c>
       <c r="G5" t="n">
-        <v>200.12</v>
+        <v>202.7321149053473</v>
       </c>
       <c r="H5" t="n">
-        <v>155.36</v>
+        <v>172.8292616669041</v>
       </c>
       <c r="I5" t="n">
-        <v>190.41</v>
+        <v>177.136238875234</v>
       </c>
       <c r="J5" t="n">
-        <v>125.08</v>
+        <v>132.8070392439114</v>
       </c>
     </row>
     <row r="6">
@@ -2167,31 +2359,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9810973293615369</v>
+        <v>0.98875853607297</v>
       </c>
       <c r="C6" t="n">
-        <v>1.011848910839918</v>
+        <v>1.023764609198471</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9924958015511011</v>
+        <v>1.001220540603886</v>
       </c>
       <c r="E6" t="n">
-        <v>281.4199999999997</v>
+        <v>286.1218068296328</v>
       </c>
       <c r="F6" t="n">
-        <v>274.91</v>
+        <v>278.5669608674862</v>
       </c>
       <c r="G6" t="n">
-        <v>200.12</v>
+        <v>202.7321149053473</v>
       </c>
       <c r="H6" t="n">
-        <v>155.36</v>
+        <v>172.8292616669041</v>
       </c>
       <c r="I6" t="n">
-        <v>190.41</v>
+        <v>177.136238875234</v>
       </c>
       <c r="J6" t="n">
-        <v>125.08</v>
+        <v>132.8070392439114</v>
       </c>
     </row>
     <row r="7">
@@ -2199,31 +2391,63 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9810972040141283</v>
+        <v>0.988758405817691</v>
       </c>
       <c r="C7" t="n">
-        <v>1.011848806191577</v>
+        <v>1.023764507135448</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9924956947825938</v>
+        <v>1.001220432367968</v>
       </c>
       <c r="E7" t="n">
-        <v>281.4199999999997</v>
+        <v>286.1218068296328</v>
       </c>
       <c r="F7" t="n">
-        <v>274.91</v>
+        <v>278.5669608674862</v>
       </c>
       <c r="G7" t="n">
-        <v>200.12</v>
+        <v>202.7321149053473</v>
       </c>
       <c r="H7" t="n">
-        <v>155.36</v>
+        <v>172.8292616669041</v>
       </c>
       <c r="I7" t="n">
-        <v>190.41</v>
+        <v>177.136238875234</v>
       </c>
       <c r="J7" t="n">
-        <v>125.08</v>
+        <v>132.8070392439114</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.9887583633869625</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.023764483853707</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.001220402689122</v>
+      </c>
+      <c r="E8" t="n">
+        <v>286.1218068296328</v>
+      </c>
+      <c r="F8" t="n">
+        <v>278.5669608674862</v>
+      </c>
+      <c r="G8" t="n">
+        <v>202.7321149053473</v>
+      </c>
+      <c r="H8" t="n">
+        <v>172.8292616669041</v>
+      </c>
+      <c r="I8" t="n">
+        <v>177.136238875234</v>
+      </c>
+      <c r="J8" t="n">
+        <v>132.8070392439114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>